<commit_message>
hope this works too
</commit_message>
<xml_diff>
--- a/sql insert generator.xlsx
+++ b/sql insert generator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="17235" windowHeight="8250" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="17235" windowHeight="8250" tabRatio="637" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="VenueLocation" sheetId="1" r:id="rId1"/>
@@ -12,17 +12,20 @@
     <sheet name="Main" sheetId="4" r:id="rId3"/>
     <sheet name="Transactions" sheetId="2" r:id="rId4"/>
     <sheet name="TransactionLine" sheetId="3" r:id="rId5"/>
-    <sheet name="Ingredient" sheetId="10" r:id="rId6"/>
-    <sheet name="MainIngredientList" sheetId="5" r:id="rId7"/>
-    <sheet name="Inventory" sheetId="6" r:id="rId8"/>
+    <sheet name="Accessories" sheetId="11" r:id="rId6"/>
+    <sheet name="ProductInventory" sheetId="12" r:id="rId7"/>
+    <sheet name="IngredientInventory" sheetId="13" r:id="rId8"/>
     <sheet name="Supply" sheetId="7" r:id="rId9"/>
+    <sheet name="MainIngredientList" sheetId="5" r:id="rId10"/>
+    <sheet name="old-ignore1" sheetId="10" r:id="rId11"/>
+    <sheet name="old-ignore" sheetId="6" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="233">
   <si>
     <t>VenueCode</t>
   </si>
@@ -700,6 +703,27 @@
   </si>
   <si>
     <t>Peach Butter</t>
+  </si>
+  <si>
+    <t>AccessoryCode</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>QuantityOnHand</t>
+  </si>
+  <si>
+    <t>Large Pie Plate</t>
+  </si>
+  <si>
+    <t>Small Pie Plate</t>
+  </si>
+  <si>
+    <t>Large  Jar</t>
+  </si>
+  <si>
+    <t>Small Jar</t>
   </si>
 </sst>
 </file>
@@ -1118,15 +1142,15 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(100, 325)</f>
-        <v>322</v>
+        <v>292</v>
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(75,150)</f>
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(20,75)</f>
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1144,15 +1168,15 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E16" ca="1" si="0">RANDBETWEEN(100, 325)</f>
-        <v>232</v>
+        <v>111</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F16" ca="1" si="1">RANDBETWEEN(75,150)</f>
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G16" ca="1" si="2">RANDBETWEEN(20,75)</f>
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1170,15 +1194,15 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>145</v>
+        <v>290</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="2"/>
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1196,15 +1220,15 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1222,15 +1246,15 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1248,15 +1272,15 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="2"/>
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1274,15 +1298,15 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>289</v>
+        <v>234</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="2"/>
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1300,15 +1324,15 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
-        <v>138</v>
+        <v>89</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="2"/>
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1326,15 +1350,15 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>274</v>
+        <v>196</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="1"/>
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="2"/>
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1352,15 +1376,15 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="1"/>
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="2"/>
-        <v>48</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1378,15 +1402,15 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>255</v>
+        <v>322</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="2"/>
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1404,15 +1428,15 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>193</v>
+        <v>306</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1430,15 +1454,15 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>146</v>
+        <v>258</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="2"/>
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1456,15 +1480,15 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>108</v>
+        <v>211</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="1"/>
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="2"/>
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1482,39 +1506,39 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>184</v>
+        <v>239</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="1"/>
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="2"/>
-        <v>63</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f ca="1">CONCATENATE("INSERT INTO venuelocation (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,", ",$E$1,", ",$F$1,", ",$G$1,") VALUES (",A2,", '",B2,"', '",C2,"', '",D2,"', '",E2,"', '",F2,"', '",G2,"');")</f>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (1, 'Trenton', '2016-03-07', '49.99', '322', '119', '58');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (1, 'Trenton', '2016-03-07', '49.99', '292', '145', '62');</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f ca="1">CONCATENATE("INSERT INTO venuelocation (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,", ",$E$1,", ",$F$1,", ",$G$1,") VALUES (",A3,", '",B3,"', '",C3,"', '",D3,"', '",E3,"', '",F3,"', '",G3,"');")</f>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (2, 'Oshawa', '2016-03-14', '60', '232', '140', '41');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (2, 'Oshawa', '2016-03-14', '60', '111', '100', '53');</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" ref="A21:A32" ca="1" si="3">CONCATENATE("INSERT INTO venuelocation (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,", ",$E$1,", ",$F$1,", ",$G$1,") VALUES (",A4,", '",B4,"', '",C4,"', '",D4,"', '",E4,"', '",F4,"', '",G4,"');")</f>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (3, 'Ajax', '2016-03-25', '44.99', '145', '128', '73');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (3, 'Ajax', '2016-03-25', '44.99', '290', '140', '60');</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (4, 'Whitby', '2016-04-01', '50', '130', '101', '20');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (4, 'Whitby', '2016-04-01', '50', '101', '128', '66');</v>
       </c>
       <c r="E22" s="2"/>
       <c r="H22" s="3"/>
@@ -1522,7 +1546,7 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (5, 'Pickering', '2016-04-08', '45', '166', '107', '25');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (5, 'Pickering', '2016-04-08', '45', '133', '85', '43');</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1530,7 +1554,7 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (6, 'Ajax', '2016-04-16', '35', '236', '93', '70');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (6, 'Ajax', '2016-04-16', '35', '204', '139', '52');</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1539,7 +1563,7 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (7, 'Oshawa', '2016-04-27', '30', '289', '136', '53');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (7, 'Oshawa', '2016-04-27', '30', '234', '97', '51');</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1547,7 +1571,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (8, 'Claremont', '2016-04-28', '20', '159', '138', '61');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (8, 'Claremont', '2016-04-28', '20', '140', '89', '44');</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1556,7 +1580,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (9, 'Toronto', '2016-05-04', '45', '274', '107', '61');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (9, 'Toronto', '2016-05-04', '45', '196', '133', '51');</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1565,7 +1589,7 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (10, 'Toronto', '2016-05-11', '49.95', '292', '146', '48');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (10, 'Toronto', '2016-05-11', '49.95', '288', '141', '28');</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1573,7 +1597,7 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (11, 'Ajax', '2016-05-17', '25', '255', '106', '68');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (11, 'Ajax', '2016-05-17', '25', '322', '97', '43');</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1582,7 +1606,7 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (12, 'Trenton', '2016-05-18', '35', '193', '91', '20');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (12, 'Trenton', '2016-05-18', '35', '306', '100', '22');</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1590,7 +1614,7 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (13, 'Whitby', '2016-05-25', '45', '146', '90', '59');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (13, 'Whitby', '2016-05-25', '45', '258', '93', '72');</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1598,7 +1622,7 @@
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (14, 'GreenWood', '2016-05-26', '50', '108', '87', '68');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (14, 'GreenWood', '2016-05-26', '50', '211', '115', '74');</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1606,7 +1630,7 @@
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f ca="1">CONCATENATE("INSERT INTO venuelocation (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,", ",$E$1,", ",$F$1,", ",$G$1,") VALUES (",A16,", '",B16,"', '",C16,"', '",D16,"', '",E16,"', '",F16,"', '",G16,"');")</f>
-        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (15, 'Markham', '2016-06-03', '50', '184', '148', '63');</v>
+        <v>INSERT INTO venuelocation (VenueCode, VenueLocation, VenueDate, VenueRentalFee, VenueFullTimeAsstCost, VenuePartTimeCost, VenueUtilityCost) VALUES (15, 'Markham', '2016-06-03', '50', '239', '103', '22');</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1789,6 +1813,587 @@
     <row r="72" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2">
+        <v>600</v>
+      </c>
+      <c r="F2">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>CONCATENATE("INSERT INTO mainingredientlist (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,", ",$E$1,", ",$F$1,", ",$G$1,") VALUES (",A2,", ",B2,", ",C2,", '",D2,"', ",E2,", ",F2,", '",G2,"');")</f>
+        <v>INSERT INTO mainingredientlist (IngredientListCode, IngredientCode, ProductCode, Description, IngredientQuantity, CostPerQuantity, IngredientUnit) VALUES (1, 1, 1, 'sample description', 600, 0.022, 'g');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4">
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6">
+        <v>11.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8">
+        <v>13.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14">
+        <v>5.49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>CONCATENATE("INSERT INTO ingredient (",$A$1,", ",$B$1,", ",$C$1,") VALUES (",A2,", '",B2,"', '",C2,"');")</f>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (1, 'Flour', '6.99');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>CONCATENATE("INSERT INTO ingredient (",$A$1,", ",$B$1,", ",$C$1,") VALUES (",A3,", '",B3,"', '",C3,"');")</f>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (2, 'Baking Soda', '3.99');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" ref="A19:A30" si="0">CONCATENATE("INSERT INTO ingredient (",$A$1,", ",$B$1,", ",$C$1,") VALUES (",A4,", '",B4,"', '",C4,"');")</f>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (3, 'Salt', '2.49');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (4, 'Sugar', '1.99');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (5, 'Steak', '11.99');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (6, 'Kidney', '4.99');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (7, 'Stout', '13.99');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (8, 'Carrots', '2.99');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (9, 'Potatoes', '3.99');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (10, 'Onion', '3.49');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (11, 'Butter', '2.99');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (12, 'Eggs', '3.29');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (13, 'Mushrooms', '5.49');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (14, 'Vegetable Oil', '4.49');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>CONCATENATE("INSERT INTO inventory (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,", ",$E$1,", ",$F$1,") VALUES (",A2,", ",B2,", '",C2,"', ",D2,", '",E2,"', '",F2,"');")</f>
+        <v>INSERT INTO inventory (InventoryID, IngredientCode, Description, QuantityInStock, InventoryUnit, CostPerUnit) VALUES (1, 1, 'Inventory table description', 5, 'Pies', '5.99');</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2345,10 +2950,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T35"/>
+  <dimension ref="A1:T53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3684,6 +4289,114 @@
         <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (2, 2, 'Pie', 'Vegetable Pie', 1000, 'TRUE', '', '', 8, 'FALSE', 500, 26, 11, 15, 7, 19, 10, 24, 10, 3);</v>
       </c>
     </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f t="shared" ref="A36:A65" si="2">CONCATENATE("INSERT INTO main (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,", ",$E$1,", ",$F$1,", ",$G$1,", ",$H$1,", ",$I$1,", ",$J$1,", ",$K$1,", ",$L$1,", ",$M$1,", ",$N$1,", ",$O$1,", ",$P$1,", ",$Q$1,", ",$R$1,", ",$S$1,", ",$T$1,") VALUES (",A4,", ",B4,", '",C4,"', '",D4,"', ",E4,", '",F4,"', '",G4,"', '",H4,"', ",I4,", '",J4,"', ",K4,", ",L4,", ",M4,", ",N4,", ",O4,", ",P4,", ",Q4,", ",R4,", ",S4,", ",T4,");")</f>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (3, 3, 'Pie', 'Beef Pie', 1000, 'TRUE', '', '', 5, 'FALSE', 450, 13, 16, 7, 2, 11, 17, 16, 12, 9);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (4, 4, 'Pie', 'Stew Pie', 1000, 'TRUE', '', '', 3, 'FALSE', 680, 16, 13, 3, 7, 18, 22, 12, 4, 17);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (5, 5, 'Pie', 'Steak and Stilton Pie', 1000, 'TRUE', '', '', 8, 'FALSE', 420, 45, 17, 50, 8, 10, 20, 15, 12, 13);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (6, 6, 'Preserve', 'Blueberry Jam', 500, 'TRUE', '', '', 2, 'FALSE', 200, 20, 11, 3, 9, 12, 22, 11, 14, 2);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (7, 7, 'Preserve', 'Strawberry Jam', 500, 'TRUE', '', '', 4, 'FALSE', 150, 26, 21, 55, 3, 29, 13, 4, 10, 3);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (8, 8, 'Preserve', 'Blackberry Jam', 500, 'TRUE', '', '', 5, 'FALSE', 160, 13, 16, 7, 2, 11, 17, 16, 12, 9);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (9, 9, 'Preserve', 'Marmalade', 500, 'TRUE', '', '', 6, 'FALSE', 180, 16, 13, 3, 7, 18, 22, 12, 4, 17);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (10, 10, 'Preserve', 'Peach Butter', 500, 'TRUE', '', '', 8, 'FALSE', 120, 15, 14, 20, 5, 30, 10, 17, 12, 13);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (11, 11, 'Pie', 'Chicken Pot Pie', 500, 'TRUE', '', '', 6, 'FALSE', 200, 10, 5, 2.5, 2.5, 5, 10, 7.5, 5, 3.5);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (12, 12, 'Pie', 'Vegetable Pie', 500, 'TRUE', '', '', 9, 'FALSE', 250, 13, 5.5, 7.5, 3.5, 9.5, 5, 12, 5, 1.5);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (13, 13, 'Pie', 'Beef Pie', 500, 'TRUE', '', '', 8, 'FALSE', 225, 6.5, 8, 3.5, 1, 5.5, 8.5, 8, 6, 4.5);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (14, 14, 'Pie', 'Stew Pie', 500, 'TRUE', '', '', 5, 'FALSE', 340, 8, 6.5, 1.5, 3.5, 9, 11, 6, 2, 8.5);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (15, 15, 'Pie', 'Steak and Stilton Pie', 500, 'TRUE', '', '', 2, 'FALSE', 210, 22.5, 8.5, 25, 4, 5, 10, 7.5, 6, 6.5);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (16, 16, 'Preserve', 'Blueberry Jam', 250, 'TRUE', '', '', 1, 'FALSE', 100, 10, 5.5, 1.5, 4.5, 6, 11, 5.5, 7, 1);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (17, 17, 'Preserve', 'Strawberry Jam', 250, 'TRUE', '', '', 2, 'FALSE', 75, 13, 10.5, 27.5, 1.5, 14.5, 6.5, 2, 5, 1.5);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (18, 18, 'Preserve', 'Blackberry Jam', 250, 'TRUE', '', '', 35, 'FALSE', 80, 6.5, 8, 3.5, 1, 5.5, 8.5, 8, 6, 4.5);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (19, 19, 'Preserve', 'Marmalade', 250, 'TRUE', '', '', 8, 'FALSE', 90, 8, 6.5, 1.5, 3.5, 9, 11, 6, 2, 8.5);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO main (ProductCode, GroupCode, ProductType, ProductName, ProductSize, Availability, ProductImageBig, ProductImageSmall, SaleAmount, OutOfProduction, Calories, Fat, SaturatedFat, TransFat, Cholesterol, Sodium, Carbohydrates, DietaryFiber, Sugar, Protein) VALUES (20, 20, 'Preserve', 'Peach Butter', 250, 'TRUE', '', '', 8, 'FALSE', 60, 7.5, 7, 10, 2.5, 15, 5, 8.5, 6, 6.5);</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3695,7 +4408,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A19" sqref="A19:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4189,10 +4902,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4489,7 +5202,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f t="shared" ref="A31:A36" si="0">CONCATENATE("INSERT INTO transactionline (",$A$1,", ",$B$1,", ",$C$1,") VALUES (",A2,", ",B2,", ",C2,");")</f>
+        <f t="shared" ref="A31:A57" si="0">CONCATENATE("INSERT INTO transactionline (",$A$1,", ",$B$1,", ",$C$1,") VALUES (",A2,", ",B2,", ",C2,");")</f>
         <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (1, 1, 3);</v>
       </c>
     </row>
@@ -4521,6 +5234,120 @@
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (6, 4, 19);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (7, 5, 3);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (8, 5, 2);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (9, 5, 11);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (10, 5, 15);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (11, 6, 20);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (12, 6, 1);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (13, 7, 8);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (14, 8, 9);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (15, 9, 6);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (16, 10, 6);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (17, 10, 7);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (18, 10, 8);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (19, 10, 9);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (20, 10, 16);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (21, 11, 18);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (22, 12, 17);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (23, 13, 15);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (24, 14, 13);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO transactionline (LineID, TransactionID, ProductCode) VALUES (25, 15, 14);</v>
       </c>
     </row>
   </sheetData>
@@ -4530,265 +5357,112 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A9" sqref="A9:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>226</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>227</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>229</v>
       </c>
       <c r="C2">
-        <v>6.99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="D2">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>230</v>
       </c>
       <c r="C3">
-        <v>3.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>231</v>
       </c>
       <c r="C4">
-        <v>2.4900000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="D4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>232</v>
       </c>
       <c r="C5">
-        <v>1.99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6">
-        <v>11.99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7">
-        <v>4.99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8">
-        <v>13.99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C9">
-        <v>2.99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10">
-        <v>3.99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11">
-        <v>3.49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>141</v>
-      </c>
-      <c r="C12">
-        <v>2.99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>142</v>
-      </c>
-      <c r="C13">
-        <v>3.29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>143</v>
-      </c>
-      <c r="C14">
-        <v>5.49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15">
-        <v>4.49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <f>CONCATENATE("INSERT INTO ingredient (",$A$1,", ",$B$1,", ",$C$1,") VALUES (",A2,", '",B2,"', '",C2,"');")</f>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (1, 'Flour', '6.99');</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
-        <f>CONCATENATE("INSERT INTO ingredient (",$A$1,", ",$B$1,", ",$C$1,") VALUES (",A3,", '",B3,"', '",C3,"');")</f>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (2, 'Baking Soda', '3.99');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
-        <f t="shared" ref="A19:A30" si="0">CONCATENATE("INSERT INTO ingredient (",$A$1,", ",$B$1,", ",$C$1,") VALUES (",A4,", '",B4,"', '",C4,"');")</f>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (3, 'Salt', '2.49');</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (4, 'Sugar', '1.99');</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (5, 'Steak', '11.99');</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (6, 'Kidney', '4.99');</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (7, 'Stout', '13.99');</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (8, 'Carrots', '2.99');</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (9, 'Potatoes', '3.99');</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (10, 'Onion', '3.49');</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (11, 'Butter', '2.99');</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (12, 'Eggs', '3.29');</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (13, 'Mushrooms', '5.49');</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO ingredient (IngredientCode, IngredientName, Cost) VALUES (14, 'Vegetable Oil', '4.49');</v>
+        <v>38</v>
+      </c>
+      <c r="D5">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>CONCATENATE("INSERT INTO accessories (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,")  VALUES (",A2,", '",B2,"', '",C2,"', '",D2,"');")</f>
+        <v>INSERT INTO accessories (AccessoryCode, Name, QuantityOnHand, CostPerUnit)  VALUES (1, 'Large Pie Plate', '67', '0.35');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" ref="A10:A12" si="0">CONCATENATE("INSERT INTO accessories (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,")  VALUES (",A3,", '",B3,"', '",C3,"', '",D3,"');")</f>
+        <v>INSERT INTO accessories (AccessoryCode, Name, QuantityOnHand, CostPerUnit)  VALUES (2, 'Small Pie Plate', '56', '0.25');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO accessories (AccessoryCode, Name, QuantityOnHand, CostPerUnit)  VALUES (3, 'Large  Jar', '44', '0.6');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO accessories (AccessoryCode, Name, QuantityOnHand, CostPerUnit)  VALUES (4, 'Small Jar', '38', '0.45');</v>
       </c>
     </row>
   </sheetData>
@@ -4798,47 +5472,34 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>226</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>228</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4846,129 +5507,416 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E2">
-        <v>600</v>
-      </c>
-      <c r="F2">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <f ca="1">RANDBETWEEN(4,55)</f>
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>6.49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C21" ca="1" si="0">RANDBETWEEN(4,55)</f>
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>6.49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>6.49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>6.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D8">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>4.79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D12">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D15">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ca="1" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D16">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ca="1" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D18">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D19">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D21">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f ca="1">CONCATENATE("INSERT INTO productinventory (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,")VALUES (",A2,", '",B2,"', '",C2,"', '",D2,"');")</f>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (1, '1', '5', '6.49');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>CONCATENATE("INSERT INTO mainingredientlist (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,", ",$E$1,", ",$F$1,", ",$G$1,") VALUES (",A2,", ",B2,", ",C2,", '",D2,"', ",E2,", ",F2,", '",G2,"');")</f>
-        <v>INSERT INTO mainingredientlist (IngredientListCode, IngredientCode, ProductCode, Description, IngredientQuantity, CostPerQuantity, IngredientUnit) VALUES (1, 1, 1, 'sample description', 600, 0.022, 'g');</v>
+        <f t="shared" ref="A25:A43" ca="1" si="1">CONCATENATE("INSERT INTO productinventory (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,")VALUES (",A3,", '",B3,"', '",C3,"', '",D3,"');")</f>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (2, '1', '40', '6.49');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (3, '1', '10', '6.99');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (4, '1', '35', '6.49');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (5, '1', '18', '6.49');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (6, '2', '22', '4.49');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (7, '2', '46', '4.49');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (8, '2', '30', '4.79');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (9, '2', '24', '4.49');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (10, '2', '17', '4.49');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (11, '3', '33', '3.49');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (12, '3', '34', '3.49');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (13, '3', '24', '3.49');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (14, '3', '25', '3.49');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (15, '3', '45', '3.49');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (16, '4', '13', '2.79');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (17, '4', '47', '2.79');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (18, '4', '41', '2.79');</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (19, '4', '25', '2.79');</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO productinventory (ProductCode, AccessoryCode, QuantityOnHand, CostPerUnit)VALUES (20, '4', '41', '2.79');</v>
       </c>
     </row>
   </sheetData>
@@ -4978,130 +5926,311 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A15"/>
+      <selection activeCell="A17" sqref="A17:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>180</v>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F2">
-        <v>5.99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>11.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>13.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13">
+        <v>48</v>
+      </c>
+      <c r="D13">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>5.49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>CONCATENATE("INSERT INTO ingredientinventory (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,") VALUES (",A2,", '",B2,"', '",C2,"', '",D2,"');")</f>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (1, 'Flour', '7', '6.99');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" ref="A18:A30" si="0">CONCATENATE("INSERT INTO ingredientinventory (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,") VALUES (",A3,", '",B3,"', '",C3,"', '",D3,"');")</f>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (2, 'Baking Soda', '4', '3.99');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (3, 'Salt', '2', '2.49');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (4, 'Sugar', '3', '1.99');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (5, 'Steak', '10', '11.99');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (6, 'Kidney', '10', '4.99');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (7, 'Stout', '8', '13.99');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (8, 'Carrots', '5', '2.99');</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>CONCATENATE("INSERT INTO inventory (",$A$1,", ",$B$1,", ",$C$1,", ",$D$1,", ",$E$1,", ",$F$1,") VALUES (",A2,", ",B2,", '",C2,"', ",D2,", '",E2,"', '",F2,"');")</f>
-        <v>INSERT INTO inventory (InventoryID, IngredientCode, Description, QuantityInStock, InventoryUnit, CostPerUnit) VALUES (1, 1, 'Inventory table description', 5, 'Pies', '5.99');</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (9, 'Potatoes', '10', '3.99');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (10, 'Onion', '7', '3.49');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (11, 'Butter', '22', '2.99');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (12, 'Eggs', '48', '3.29');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (13, 'Mushrooms', '5', '5.49');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ingredientinventory (IngredientCode, IngredientName, QuantityOnHand, CostPerUnit) VALUES (14, 'Vegetable Oil', '3', '4.49');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
most recent excel table reflecting the changes from today
</commit_message>
<xml_diff>
--- a/sql insert generator.xlsx
+++ b/sql insert generator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="17235" windowHeight="8250" tabRatio="637" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="17235" windowHeight="8250" tabRatio="637" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="VenueLocation" sheetId="1" r:id="rId1"/>
@@ -1823,7 +1823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -2003,7 +2003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>